<commit_message>
agregamos el Archivo de Backlog de producto, de producto detallado y del Sprint
</commit_message>
<xml_diff>
--- a/Backlog del Producto.xlsx
+++ b/Backlog del Producto.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\MAESTRIA UNH\proyecto\proyecto-01\PlantillasGP\Plantillas de Gestión de Proyecto\01. INICIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CJARA\Desktop\proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1C2622-52B1-4A18-9567-7B6D40CFD282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="522" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="522"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog del Producto" sheetId="8" r:id="rId1"/>
@@ -31,13 +30,13 @@
     <definedName name="PBCurrentBottom">OFFSET(#REF!,1,0,#REF!,1)</definedName>
     <definedName name="PBTrend">OFFSET(#REF!,1,0,#REF!,1)</definedName>
     <definedName name="PlannedSpeed">OFFSET(#REF!,1,0,#REF!,1)</definedName>
-    <definedName name="ProductBacklog">'Backlog del Producto'!$B$5:$P$190</definedName>
+    <definedName name="ProductBacklog">'Backlog del Producto'!$B$5:$P$195</definedName>
     <definedName name="RealizedSpeed">OFFSET(#REF!,1,0,#REF!,1)</definedName>
-    <definedName name="Sprint">'Backlog del Producto'!$N$7:$N$190</definedName>
+    <definedName name="Sprint">'Backlog del Producto'!$N$12:$N$195</definedName>
     <definedName name="SprintCount">#REF!</definedName>
     <definedName name="SprintsInTrend">#REF!</definedName>
     <definedName name="SprintTasks">#REF!</definedName>
-    <definedName name="Status">'Backlog del Producto'!$O$7:$O$190</definedName>
+    <definedName name="Status">'Backlog del Producto'!$O$12:$O$195</definedName>
     <definedName name="StoryName">'Backlog del Producto'!#REF!</definedName>
     <definedName name="TaskRows">#REF!</definedName>
     <definedName name="TaskStatus">#REF!</definedName>
@@ -47,7 +46,7 @@
     <definedName name="TrendOffset">#REF!</definedName>
     <definedName name="TrendSprintCount">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -62,14 +61,14 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hector Bravo Consultor GE</author>
     <author>Petri Heiramo</author>
     <author>Hector Bravo</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -82,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="F6" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -95,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="K6" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -109,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="L6" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="M6" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="N6" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="O6" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -187,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
   <si>
     <t>Sprint</t>
   </si>
@@ -306,25 +305,10 @@
     <t>Dependencias</t>
   </si>
   <si>
-    <t>Poder generar reportes de estudiantes que desertaron de la facultad de ingenieria</t>
-  </si>
-  <si>
     <t>Presentar la buena toma de desiciones</t>
   </si>
   <si>
     <t>Cientifico de datos</t>
-  </si>
-  <si>
-    <t>Deseo poder generar el reporte de estudiantes desertados de la carrera profesional de ingenieria de sistemas e informatica</t>
-  </si>
-  <si>
-    <t>Deseo generar el reporte de estudiantes desertados de la carrera profesional de ingenieria forestal y medio ambiente</t>
-  </si>
-  <si>
-    <t>Deseo poder generar el reporte de estudiantes desertados de la carrera de ingenieria agroidustrial</t>
-  </si>
-  <si>
-    <t>Deseo poder generar el reporte de estudiantes desertados de la carrera de mediciona veterinaria y zootecnia</t>
   </si>
   <si>
     <t>Presentar la situación de desertores al Director de DUAA</t>
@@ -346,9 +330,6 @@
     <t>Tomar medidas preventivas y correctivas sobre la desercion universitaria</t>
   </si>
   <si>
-    <t>Director de DUAA</t>
-  </si>
-  <si>
     <t>Generar dashboard de estados estadisticos de desercion de estudiantes de la facultad de ingenieria</t>
   </si>
   <si>
@@ -383,12 +364,93 @@
   </si>
   <si>
     <t>El cliente este conforme con los resultados</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Poder ingresar con un login al sistema</t>
+  </si>
+  <si>
+    <t>para ingresar al sitema</t>
+  </si>
+  <si>
+    <t>Crear pantalla de login</t>
+  </si>
+  <si>
+    <t>Crear cajas de texto para los campos nombre de usuario y clave</t>
+  </si>
+  <si>
+    <t>Crear la consulta a la base de datos para validad el nombre de usuario y clave</t>
+  </si>
+  <si>
+    <t>Determinar si el requerimiento del login fue exitoso o fallo</t>
+  </si>
+  <si>
+    <t>Recuperar contraseña</t>
+  </si>
+  <si>
+    <t>la interfaz</t>
+  </si>
+  <si>
+    <t>para el registro de usuario</t>
+  </si>
+  <si>
+    <t>conectarse con la base de datos</t>
+  </si>
+  <si>
+    <t>para validar el ingreso</t>
+  </si>
+  <si>
+    <t>para que los usuarios puedan ingresar de nuevo</t>
+  </si>
+  <si>
+    <t>Recuperacion de contraseña por correo electronico</t>
+  </si>
+  <si>
+    <t>Debe ser responsive</t>
+  </si>
+  <si>
+    <t>Los campos obligatorios</t>
+  </si>
+  <si>
+    <t>Colocar una seguridad de verificacion de bots, como recaptcha</t>
+  </si>
+  <si>
+    <t>HU07</t>
+  </si>
+  <si>
+    <t>HU08</t>
+  </si>
+  <si>
+    <t>HU09</t>
+  </si>
+  <si>
+    <t>HU10</t>
+  </si>
+  <si>
+    <t>EPIC05</t>
+  </si>
+  <si>
+    <t>Poder predecir los estudiantes que desertaron de la facultad de ingenieria</t>
+  </si>
+  <si>
+    <t>Deseo poder predecir los estudiantes desertados de la carrera profesional de ingenieria de sistemas e informatica</t>
+  </si>
+  <si>
+    <t>Deseo poder predecir los  estudiantes desertados de la carrera profesional de ingenieria forestal y medio ambiente</t>
+  </si>
+  <si>
+    <t>Deseo poder predecir los  estudiantes desertados de la carrera de ingenieria agroidustrial</t>
+  </si>
+  <si>
+    <t>Deseo poder predecir los estudiantes desertados de la carrera de mediciona veterinaria y zootecnia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -455,7 +517,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,6 +569,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -667,9 +735,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -694,8 +759,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -729,15 +827,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="37">
     <dxf>
       <font>
         <b/>
@@ -789,6 +884,94 @@
         <extend val="0"/>
         <color indexed="54"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor indexed="10"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1306,14 +1489,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:S80"/>
+  <dimension ref="B1:S85"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1350,23 +1533,23 @@
       </c>
     </row>
     <row r="2" spans="2:19" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="65"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
       <c r="O2" s="30"/>
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
@@ -1376,23 +1559,23 @@
       </c>
     </row>
     <row r="3" spans="2:19" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="65"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
       <c r="O3" s="30"/>
       <c r="P3" s="24"/>
       <c r="Q3" s="24"/>
@@ -1424,27 +1607,27 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48" t="s">
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="51" t="s">
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="53"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="63"/>
     </row>
     <row r="6" spans="2:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="34" t="s">
@@ -1459,323 +1642,329 @@
       <c r="E6" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="40" t="s">
+      <c r="K6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="40" t="s">
+      <c r="L6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="40" t="s">
+      <c r="M6" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="40" t="s">
+      <c r="N6" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="O6" s="40" t="s">
+      <c r="O6" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="39" t="s">
+      <c r="P6" s="38" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="42" t="s">
+    <row r="7" spans="2:19" s="47" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="9"/>
-    </row>
-    <row r="8" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42" t="s">
+      <c r="C7" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J8" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="K8" s="8">
+      <c r="G7" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="45">
         <v>1</v>
       </c>
-      <c r="L8" s="8">
-        <v>25</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8">
+      <c r="L7" s="45">
+        <v>10</v>
+      </c>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45"/>
+      <c r="O7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P7" s="46"/>
+    </row>
+    <row r="8" spans="2:19" s="47" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="46"/>
+      <c r="H8" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="45">
         <v>1</v>
       </c>
+      <c r="L8" s="45">
+        <v>10</v>
+      </c>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
       <c r="O8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="9"/>
-    </row>
-    <row r="9" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42" t="s">
+      <c r="P8" s="46"/>
+    </row>
+    <row r="9" spans="2:19" s="47" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="46"/>
+      <c r="H9" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="48"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45">
+        <v>5</v>
+      </c>
+      <c r="M9" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="I9" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" s="8">
-        <v>1</v>
-      </c>
-      <c r="L9" s="8">
-        <v>25</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8">
-        <v>1</v>
-      </c>
+      <c r="N9" s="45"/>
       <c r="O9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="9"/>
-    </row>
-    <row r="10" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="42" t="s">
+      <c r="P9" s="46"/>
+    </row>
+    <row r="10" spans="2:19" s="47" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="46"/>
+      <c r="H10" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="45">
+        <v>2</v>
+      </c>
+      <c r="L10" s="45">
+        <v>10</v>
+      </c>
+      <c r="M10" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="8">
-        <v>1</v>
-      </c>
-      <c r="L10" s="8">
-        <v>20</v>
-      </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8">
-        <v>2</v>
-      </c>
+      <c r="N10" s="45"/>
       <c r="O10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P10" s="9"/>
-    </row>
-    <row r="11" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="K11" s="8">
+      <c r="P10" s="46"/>
+    </row>
+    <row r="11" spans="2:19" s="47" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="46"/>
+      <c r="H11" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="I11" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="K11" s="45">
         <v>1</v>
       </c>
-      <c r="L11" s="8">
-        <v>15</v>
-      </c>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8">
-        <v>2</v>
-      </c>
+      <c r="L11" s="45">
+        <v>10</v>
+      </c>
+      <c r="M11" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="45"/>
       <c r="O11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P11" s="9"/>
-    </row>
-    <row r="12" spans="2:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="43" t="s">
+      <c r="P11" s="46"/>
+    </row>
+    <row r="12" spans="2:19" s="54" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="9"/>
-    </row>
-    <row r="13" spans="2:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="42" t="s">
+      <c r="C12" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="50"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49">
+        <v>27</v>
+      </c>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="53"/>
+    </row>
+    <row r="13" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+      <c r="G13" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="8">
+        <v>1</v>
+      </c>
+      <c r="L13" s="8">
+        <v>21</v>
+      </c>
       <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
+      <c r="N13" s="8">
+        <v>1</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P13" s="9"/>
     </row>
-    <row r="14" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="42" t="s">
-        <v>46</v>
+    <row r="14" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="41" t="s">
+        <v>39</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K14" s="8">
         <v>1</v>
       </c>
       <c r="L14" s="8">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O14" s="8" t="s">
         <v>11</v>
       </c>
       <c r="P14" s="9"/>
     </row>
-    <row r="15" spans="2:19" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B15" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" s="42" t="s">
-        <v>62</v>
+    <row r="15" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="41" t="s">
+        <v>39</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="K15" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L15" s="8">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M15" s="8"/>
       <c r="N15" s="8">
@@ -1786,32 +1975,58 @@
       </c>
       <c r="P15" s="9"/>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:19" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B16" s="42"/>
       <c r="C16" s="42"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="8">
+        <v>1</v>
+      </c>
+      <c r="L16" s="8">
+        <v>20</v>
+      </c>
       <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
+      <c r="N16" s="8">
+        <v>2</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P16" s="9"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+    <row r="17" spans="2:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="9"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
@@ -1820,15 +2035,23 @@
       <c r="O17" s="8"/>
       <c r="P17" s="9"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
+    <row r="18" spans="2:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="9"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
@@ -1837,49 +2060,93 @@
       <c r="O18" s="8"/>
       <c r="P18" s="9"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+    <row r="19" spans="2:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="8">
+        <v>1</v>
+      </c>
+      <c r="L19" s="8">
+        <v>25</v>
+      </c>
       <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
+      <c r="N19" s="8">
+        <v>2</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P19" s="9"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
+    <row r="20" spans="2:16" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B20" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="8">
+        <v>2</v>
+      </c>
+      <c r="L20" s="8">
+        <v>15</v>
+      </c>
       <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
+      <c r="N20" s="8">
+        <v>2</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="P20" s="9"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
       <c r="J21" s="9"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
@@ -1889,14 +2156,14 @@
       <c r="P21" s="9"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
       <c r="J22" s="9"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
@@ -1906,14 +2173,14 @@
       <c r="P22" s="9"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
       <c r="J23" s="9"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
@@ -1923,14 +2190,14 @@
       <c r="P23" s="9"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
       <c r="J24" s="9"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
@@ -1940,14 +2207,14 @@
       <c r="P24" s="9"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
       <c r="J25" s="9"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
@@ -1957,14 +2224,14 @@
       <c r="P25" s="9"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="42"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
       <c r="J26" s="9"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
@@ -1974,14 +2241,14 @@
       <c r="P26" s="9"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
       <c r="J27" s="9"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
@@ -1991,14 +2258,14 @@
       <c r="P27" s="9"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
       <c r="J28" s="9"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
@@ -2008,14 +2275,14 @@
       <c r="P28" s="9"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
       <c r="J29" s="9"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
@@ -2025,14 +2292,14 @@
       <c r="P29" s="9"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
       <c r="J30" s="9"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
@@ -2042,14 +2309,14 @@
       <c r="P30" s="9"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
       <c r="J31" s="9"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
@@ -2059,14 +2326,14 @@
       <c r="P31" s="9"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
       <c r="J32" s="9"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
@@ -2076,14 +2343,14 @@
       <c r="P32" s="9"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
       <c r="J33" s="9"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
@@ -2093,14 +2360,14 @@
       <c r="P33" s="9"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
       <c r="J34" s="9"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
@@ -2110,14 +2377,14 @@
       <c r="P34" s="9"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
       <c r="J35" s="9"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
@@ -2127,14 +2394,14 @@
       <c r="P35" s="9"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
       <c r="J36" s="9"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
@@ -2144,14 +2411,14 @@
       <c r="P36" s="9"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
       <c r="J37" s="9"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
@@ -2161,14 +2428,14 @@
       <c r="P37" s="9"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="43"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
       <c r="J38" s="9"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
@@ -2178,14 +2445,14 @@
       <c r="P38" s="9"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="43"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="43"/>
-      <c r="H39" s="43"/>
-      <c r="I39" s="43"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
       <c r="J39" s="9"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
@@ -2195,14 +2462,14 @@
       <c r="P39" s="9"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
       <c r="J40" s="9"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
@@ -2212,14 +2479,14 @@
       <c r="P40" s="9"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
       <c r="J41" s="9"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
@@ -2229,14 +2496,14 @@
       <c r="P41" s="9"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
       <c r="J42" s="9"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
@@ -2246,14 +2513,14 @@
       <c r="P42" s="9"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
       <c r="J43" s="9"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
@@ -2263,14 +2530,14 @@
       <c r="P43" s="9"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
+      <c r="E44" s="42"/>
+      <c r="F44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
       <c r="J44" s="9"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
@@ -2280,14 +2547,14 @@
       <c r="P44" s="9"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="43"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="43"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
       <c r="J45" s="9"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
@@ -2297,14 +2564,14 @@
       <c r="P45" s="9"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
       <c r="J46" s="9"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
@@ -2314,14 +2581,14 @@
       <c r="P46" s="9"/>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="42"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="42"/>
       <c r="J47" s="9"/>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
@@ -2331,14 +2598,14 @@
       <c r="P47" s="9"/>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
       <c r="J48" s="9"/>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
@@ -2348,14 +2615,14 @@
       <c r="P48" s="9"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
+      <c r="B49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="42"/>
+      <c r="H49" s="42"/>
+      <c r="I49" s="42"/>
       <c r="J49" s="9"/>
       <c r="K49" s="8"/>
       <c r="L49" s="8"/>
@@ -2365,14 +2632,14 @@
       <c r="P49" s="9"/>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
       <c r="J50" s="9"/>
       <c r="K50" s="8"/>
       <c r="L50" s="8"/>
@@ -2382,14 +2649,14 @@
       <c r="P50" s="9"/>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
+      <c r="B51" s="42"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="42"/>
       <c r="J51" s="9"/>
       <c r="K51" s="8"/>
       <c r="L51" s="8"/>
@@ -2398,30 +2665,115 @@
       <c r="O51" s="8"/>
       <c r="P51" s="9"/>
     </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="F52" s="42"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="42"/>
+      <c r="I52" s="42"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="9"/>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B53" s="42"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="42"/>
+      <c r="G53" s="42"/>
+      <c r="H53" s="42"/>
+      <c r="I53" s="42"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="9"/>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="42"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="9"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B55" s="42"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
+      <c r="H55" s="42"/>
+      <c r="I55" s="42"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="9"/>
+    </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="G56" s="6"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-    </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P69" s="7"/>
-    </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-      <c r="G80" s="6"/>
-      <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
-      <c r="J80" s="6"/>
-      <c r="K80" s="6"/>
-      <c r="L80" s="6"/>
-      <c r="M80" s="6"/>
-      <c r="N80" s="6"/>
-      <c r="O80" s="6"/>
+      <c r="B56" s="42"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="42"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="42"/>
+      <c r="H56" s="42"/>
+      <c r="I56" s="42"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="9"/>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+    </row>
+    <row r="74" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P74" s="7"/>
+    </row>
+    <row r="85" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2434,77 +2786,121 @@
     <mergeCell ref="D3:E3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="P69:P70">
-    <cfRule type="expression" dxfId="24" priority="25" stopIfTrue="1">
+  <conditionalFormatting sqref="P74:P75">
+    <cfRule type="expression" dxfId="36" priority="37" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="38" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="39" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P24">
-    <cfRule type="expression" dxfId="21" priority="28" stopIfTrue="1">
+  <conditionalFormatting sqref="P29">
+    <cfRule type="expression" dxfId="33" priority="40" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="41" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="42" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P80">
-    <cfRule type="expression" dxfId="18" priority="73" stopIfTrue="1">
-      <formula>$O70="Done"</formula>
+  <conditionalFormatting sqref="P85">
+    <cfRule type="expression" dxfId="30" priority="85" stopIfTrue="1">
+      <formula>$O75="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="74" stopIfTrue="1">
-      <formula>$O70="Ongoing"</formula>
+    <cfRule type="expression" dxfId="29" priority="86" stopIfTrue="1">
+      <formula>$O75="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="75" stopIfTrue="1">
-      <formula>$O70="Removed"</formula>
+    <cfRule type="expression" dxfId="28" priority="87" stopIfTrue="1">
+      <formula>$O75="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7 K7:P125 B7:G7 B8:J125">
-    <cfRule type="expression" dxfId="15" priority="31" stopIfTrue="1">
+  <conditionalFormatting sqref="I12 B13:E16 B17:P130 K12:K16 M12:P16 B12 G12:G16 G13:J16">
+    <cfRule type="expression" dxfId="27" priority="43" stopIfTrue="1">
+      <formula>$O12="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="44" stopIfTrue="1">
+      <formula>$O12="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="45" stopIfTrue="1">
+      <formula>$O12="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R3">
+    <cfRule type="expression" dxfId="24" priority="91" stopIfTrue="1">
+      <formula>$O16="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="23" priority="92" stopIfTrue="1">
+      <formula>$O16="In Progress"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="93" stopIfTrue="1">
+      <formula>$O16="Removed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1">
+    <cfRule type="expression" dxfId="21" priority="94" stopIfTrue="1">
+      <formula>$O14="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="95" stopIfTrue="1">
+      <formula>$O14="In Progress"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="96" stopIfTrue="1">
+      <formula>$O14="Removed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O7:O11">
+    <cfRule type="expression" dxfId="18" priority="10" stopIfTrue="1">
       <formula>$O7="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="11" stopIfTrue="1">
       <formula>$O7="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="12" stopIfTrue="1">
       <formula>$O7="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R3">
-    <cfRule type="expression" dxfId="12" priority="79" stopIfTrue="1">
-      <formula>$O11="Done"</formula>
+  <conditionalFormatting sqref="L12:L16">
+    <cfRule type="expression" dxfId="15" priority="7" stopIfTrue="1">
+      <formula>$O12="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="80" stopIfTrue="1">
-      <formula>$O11="In Progress"</formula>
+    <cfRule type="expression" dxfId="14" priority="8" stopIfTrue="1">
+      <formula>$O12="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="81" stopIfTrue="1">
-      <formula>$O11="Removed"</formula>
+    <cfRule type="expression" dxfId="13" priority="9" stopIfTrue="1">
+      <formula>$O12="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1">
-    <cfRule type="expression" dxfId="9" priority="82" stopIfTrue="1">
-      <formula>$O9="Done"</formula>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="12" priority="4" stopIfTrue="1">
+      <formula>$O12="Terminado"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="83" stopIfTrue="1">
-      <formula>$O9="In Progress"</formula>
+    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
+      <formula>$O12="En Progreso"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="84" stopIfTrue="1">
-      <formula>$O9="Removed"</formula>
+    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
+      <formula>$O12="Eliminado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12:E12">
+    <cfRule type="expression" dxfId="9" priority="1" stopIfTrue="1">
+      <formula>$O12="Terminado"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="2" stopIfTrue="1">
+      <formula>$O12="En Progreso"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+      <formula>$O12="Eliminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="O81:O190 O6:O79" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="O86:O195 O6:O84">
       <formula1>"Por Hacer,En Progreso,Terminado,Eliminado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K51" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K12:K56">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2516,7 +2912,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:J18"/>
   <sheetViews>
@@ -2570,7 +2966,7 @@
       <c r="B3" s="17">
         <v>1</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="36">
         <v>44732</v>
       </c>
       <c r="D3" s="20">
@@ -2580,15 +2976,15 @@
         <v>43362</v>
       </c>
       <c r="F3" s="17">
-        <f>IF(B3="","",SUMIF('Backlog del Producto'!N$7:N$130,Sprints!B3,'Backlog del Producto'!L$7:L$130))</f>
-        <v>50</v>
+        <f>IF(B3="","",SUMIF('Backlog del Producto'!N$12:N$135,Sprints!B3,'Backlog del Producto'!L$12:L$135))</f>
+        <v>42</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="20"/>
-      <c r="I3" s="56" t="s">
-        <v>64</v>
+      <c r="I3" s="43" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -2607,15 +3003,15 @@
         <v>44791</v>
       </c>
       <c r="F4" s="17">
-        <f>IF(B4="","",SUMIF('Backlog del Producto'!N$7:N$130,Sprints!B4,'Backlog del Producto'!L$7:L$130))</f>
-        <v>75</v>
+        <f>IF(B4="","",SUMIF('Backlog del Producto'!N$12:N$135,Sprints!B4,'Backlog del Producto'!L$12:L$135))</f>
+        <v>81</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="20"/>
-      <c r="I4" s="56" t="s">
-        <v>64</v>
+      <c r="I4" s="43" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
@@ -2634,7 +3030,7 @@
         <v>44821</v>
       </c>
       <c r="F5" s="17">
-        <f>IF(B5="","",SUMIF('Backlog del Producto'!N$7:N$130,Sprints!B5,'Backlog del Producto'!L$7:L$130))</f>
+        <f>IF(B5="","",SUMIF('Backlog del Producto'!N$12:N$135,Sprints!B5,'Backlog del Producto'!L$12:L$135))</f>
         <v>0</v>
       </c>
       <c r="G5" s="18" t="s">
@@ -2659,7 +3055,7 @@
         <v>44851</v>
       </c>
       <c r="F6" s="17">
-        <f>IF(B6="","",SUMIF('Backlog del Producto'!N$7:N$130,Sprints!B6,'Backlog del Producto'!L$7:L$130))</f>
+        <f>IF(B6="","",SUMIF('Backlog del Producto'!N$12:N$135,Sprints!B6,'Backlog del Producto'!L$12:L$135))</f>
         <v>0</v>
       </c>
       <c r="G6" s="18" t="s">
@@ -2684,7 +3080,7 @@
         <v>44881</v>
       </c>
       <c r="F7" s="17">
-        <f>IF(B7="","",SUMIF('Backlog del Producto'!N$7:N$130,Sprints!B7,'Backlog del Producto'!L$7:L$130))</f>
+        <f>IF(B7="","",SUMIF('Backlog del Producto'!N$12:N$135,Sprints!B7,'Backlog del Producto'!L$12:L$135))</f>
         <v>0</v>
       </c>
       <c r="G7" s="18" t="s">
@@ -2718,7 +3114,7 @@
         <v/>
       </c>
       <c r="F9" s="17" t="str">
-        <f>IF(B9="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B9,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B9="","",SUMIF('Backlog del Producto'!N$13:N$135,Sprints!B9,'Backlog del Producto'!L$13:L$135))</f>
         <v/>
       </c>
       <c r="G9" s="18" t="str">
@@ -2743,7 +3139,7 @@
         <v/>
       </c>
       <c r="F10" s="17" t="str">
-        <f>IF(B10="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B10,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B10="","",SUMIF('Backlog del Producto'!N$13:N$135,Sprints!B10,'Backlog del Producto'!L$13:L$135))</f>
         <v/>
       </c>
       <c r="G10" s="18" t="str">
@@ -2768,7 +3164,7 @@
         <v/>
       </c>
       <c r="F11" s="17" t="str">
-        <f>IF(B11="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B11,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B11="","",SUMIF('Backlog del Producto'!N$13:N$135,Sprints!B11,'Backlog del Producto'!L$13:L$135))</f>
         <v/>
       </c>
       <c r="G11" s="18" t="str">
@@ -2793,7 +3189,7 @@
         <v/>
       </c>
       <c r="F12" s="17" t="str">
-        <f>IF(B12="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B12,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B12="","",SUMIF('Backlog del Producto'!N$13:N$135,Sprints!B12,'Backlog del Producto'!L$13:L$135))</f>
         <v/>
       </c>
       <c r="G12" s="18" t="str">
@@ -2818,7 +3214,7 @@
         <v/>
       </c>
       <c r="F13" s="17" t="str">
-        <f>IF(B13="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B13,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B13="","",SUMIF('Backlog del Producto'!N$13:N$135,Sprints!B13,'Backlog del Producto'!L$13:L$135))</f>
         <v/>
       </c>
       <c r="G13" s="18" t="str">
@@ -2843,7 +3239,7 @@
         <v/>
       </c>
       <c r="F14" s="17" t="str">
-        <f>IF(B14="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B14,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B14="","",SUMIF('Backlog del Producto'!N$13:N$135,Sprints!B14,'Backlog del Producto'!L$13:L$135))</f>
         <v/>
       </c>
       <c r="G14" s="18" t="str">
@@ -2868,7 +3264,7 @@
         <v/>
       </c>
       <c r="F15" s="17" t="str">
-        <f>IF(B15="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B15,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B15="","",SUMIF('Backlog del Producto'!N$13:N$135,Sprints!B15,'Backlog del Producto'!L$13:L$135))</f>
         <v/>
       </c>
       <c r="G15" s="18" t="str">
@@ -2893,7 +3289,7 @@
         <v/>
       </c>
       <c r="F16" s="17" t="str">
-        <f>IF(B16="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B16,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B16="","",SUMIF('Backlog del Producto'!N$13:N$135,Sprints!B16,'Backlog del Producto'!L$13:L$135))</f>
         <v/>
       </c>
       <c r="G16" s="18" t="str">
@@ -2918,7 +3314,7 @@
         <v/>
       </c>
       <c r="F17" s="17" t="str">
-        <f>IF(B17="","",SUMIF('Backlog del Producto'!N$8:N$130,Sprints!B17,'Backlog del Producto'!L$8:L$130))</f>
+        <f>IF(B17="","",SUMIF('Backlog del Producto'!N$13:N$135,Sprints!B17,'Backlog del Producto'!L$13:L$135))</f>
         <v/>
       </c>
       <c r="G17" s="18" t="str">
@@ -2936,7 +3332,7 @@
         <v>14</v>
       </c>
       <c r="F18" s="17">
-        <f>SUMIF('Backlog del Producto'!N$8:N$130,"",'Backlog del Producto'!L$8:L$130)-SUMIF('Backlog del Producto'!O$8:O$130,"Eliminado",'Backlog del Producto'!L$8:L$130)</f>
+        <f>SUMIF('Backlog del Producto'!N$13:N$135,"",'Backlog del Producto'!L$13:L$135)-SUMIF('Backlog del Producto'!O$13:O$135,"Eliminado",'Backlog del Producto'!L$13:L$135)</f>
         <v>0</v>
       </c>
       <c r="G18" s="18"/>
@@ -2973,7 +3369,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G17" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G17">
       <formula1>"Planeado,En Progreso,Terminado,No planeado"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2984,12 +3380,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2998,7 +3398,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5124E24CAF14D46B2DD609ACFD84C07" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9971b3b784abbe199b171e233c6d3889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a36e787f936117f0a8f63b0cc0186e7" ns2:_="">
     <xsd:import namespace="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a"/>
@@ -3143,7 +3543,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -3193,27 +3593,31 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A0D1E8-B670-4184-80F1-6022252F7605}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A0D1E8-B670-4184-80F1-6022252F7605}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="01eb4bd6-a8ff-4439-b7eb-fe0a650fbd8a"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2036E817-ADB2-4FBD-A97A-810F82FD54C5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -3221,7 +3625,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617ABD26-2811-4761-B5CB-14D5621085A8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3239,18 +3643,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F09A1246-53BD-4D90-8F0D-F04270C7DF7F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2926A6BD-B9D6-43A1-AC24-40D994CC1A5B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>